<commit_message>
indicadores económicos en Python
Trabaje con el calculo de indicadores economicos.py
</commit_message>
<xml_diff>
--- a/Base de datos Python/Base datos Arreglada/Base_Datos_2001.xlsx
+++ b/Base de datos Python/Base datos Arreglada/Base_Datos_2001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose Inestroza\Documents\GitHub\Proyecto_investigacion_semiario\Base de datos Python\Base datos Arreglada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FD5CE0-7F33-4179-A7EB-FB6BE74E70EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96779D1-4B52-4A50-8F5A-918FAA9E698D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0048E4E5-1594-4D40-96C3-2DEB681BC601}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Calculo del modelo AR y Auto covarianza Python y Excel
Calculo del modelo AR y auto covarianza
Python Excel
</commit_message>
<xml_diff>
--- a/Base de datos Python/Base datos Arreglada/Base_Datos_2001.xlsx
+++ b/Base de datos Python/Base datos Arreglada/Base_Datos_2001.xlsx
@@ -8,70 +8,72 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose Inestroza\Documents\GitHub\Proyecto_investigacion_semiario\Base de datos Python\Base datos Arreglada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A63E6BD-31EA-4D7D-A2B6-2DA00946E141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D346F8E-C110-4557-8DF6-BFC75F846C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{0048E4E5-1594-4D40-96C3-2DEB681BC601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{0048E4E5-1594-4D40-96C3-2DEB681BC601}"/>
   </bookViews>
   <sheets>
     <sheet name="BASE DATOS 2001 Y 2013 " sheetId="1" r:id="rId1"/>
     <sheet name="Modelo AR" sheetId="2" r:id="rId2"/>
-    <sheet name="Modelo ARMA(1,1)" sheetId="3" r:id="rId3"/>
+    <sheet name="Suavisacion de los datos " sheetId="4" r:id="rId3"/>
+    <sheet name="Base_Datos_Suavisada_2001_2013" sheetId="5" r:id="rId4"/>
+    <sheet name="Modelo ARMA(1,1)" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="1" hidden="1">'Modelo AR'!$K$7:$K$8</definedName>
-    <definedName name="solver_adj" localSheetId="2" hidden="1">'Modelo ARMA(1,1)'!$K$7:$K$9</definedName>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">'Modelo ARMA(1,1)'!$K$7:$K$9</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
-    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
-    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
-    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_num" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">'Modelo AR'!$K$11</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">'Modelo ARMA(1,1)'!$K$11</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">'Modelo ARMA(1,1)'!$K$11</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
-    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
-    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
-    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -83,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="88">
   <si>
     <t xml:space="preserve">Departamento </t>
   </si>
@@ -305,6 +307,70 @@
   </si>
   <si>
     <t>2. Lo ideal es quedarse con el metodo donde el "Error"es el valor mas pequeño</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antes </t>
+  </si>
+  <si>
+    <t>Antes</t>
+  </si>
+  <si>
+    <t>Promedios_moviles_Ocupados_H</t>
+  </si>
+  <si>
+    <t>Promedios_Moviles_Ocupados_M</t>
+  </si>
+  <si>
+    <t>Promedios_Moviles_Ocupados_Total</t>
+  </si>
+  <si>
+    <t>Promedios_Moviles_Desocupados_H</t>
+  </si>
+  <si>
+    <t>Promedios_Moviles_Desocupados_M</t>
+  </si>
+  <si>
+    <t>Promedios_Moviles_Des_Total</t>
+  </si>
+  <si>
+    <t>Promedios_Moviles_Inac_H</t>
+  </si>
+  <si>
+    <t>Promedios_Moviles_Inac_M</t>
+  </si>
+  <si>
+    <t>Promedios_Moviles_Inac_T</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ecua: c+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>α1*(Yt-1)+Et</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>AR1=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>α1*(Yt-1)+Et</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -313,11 +379,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +397,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -434,7 +512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -446,11 +524,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -769,7 +848,7 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A37"/>
+      <selection activeCell="B1" sqref="B1:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2427,7 +2506,7 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C42"/>
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2670,6 +2749,9 @@
         <f t="shared" si="2"/>
         <v>7946973682.7092381</v>
       </c>
+      <c r="M10" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2732,6 +2814,9 @@
         <f t="shared" si="2"/>
         <v>214423302.12209553</v>
       </c>
+      <c r="M12" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2784,6 +2869,9 @@
         <f t="shared" si="2"/>
         <v>702525619.58630943</v>
       </c>
+      <c r="K14" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -2810,6 +2898,12 @@
         <f t="shared" si="2"/>
         <v>521537697.41781032</v>
       </c>
+      <c r="K15" t="s">
+        <v>63</v>
+      </c>
+      <c r="L15">
+        <v>1.1000000000000001</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2836,6 +2930,12 @@
         <f t="shared" si="2"/>
         <v>793165826.3200531</v>
       </c>
+      <c r="K16" t="s">
+        <v>64</v>
+      </c>
+      <c r="L16">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -3495,7 +3595,10 @@
         <f t="shared" si="0"/>
         <v>30972.19985939192</v>
       </c>
-      <c r="H42" s="12"/>
+      <c r="H42" s="12">
+        <f>SUM(H7:H41)</f>
+        <v>70554486749.600006</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
@@ -3508,11 +3611,3521 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5FC4F1B-9191-446A-B33B-F26232C49C55}">
+  <dimension ref="C1:Q37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="33" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" customWidth="1"/>
+    <col min="9" max="9" width="36" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" customWidth="1"/>
+    <col min="11" max="11" width="34.5703125" customWidth="1"/>
+    <col min="12" max="12" width="28.5703125" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" customWidth="1"/>
+    <col min="14" max="14" width="27.140625" customWidth="1"/>
+    <col min="15" max="15" width="21" customWidth="1"/>
+    <col min="16" max="16" width="28.140625" customWidth="1"/>
+    <col min="17" max="17" width="26.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C2" s="1">
+        <v>66929</v>
+      </c>
+      <c r="D2" s="1">
+        <v>66929</v>
+      </c>
+      <c r="E2" s="1">
+        <v>21562</v>
+      </c>
+      <c r="F2" s="1">
+        <v>21562</v>
+      </c>
+      <c r="G2" s="14">
+        <f>(D2+F2)</f>
+        <v>88491</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1606</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1606</v>
+      </c>
+      <c r="J2" s="1">
+        <v>417</v>
+      </c>
+      <c r="K2" s="1">
+        <v>417</v>
+      </c>
+      <c r="L2" s="14">
+        <f>(I2+K2)</f>
+        <v>2023</v>
+      </c>
+      <c r="M2" s="1">
+        <v>56224</v>
+      </c>
+      <c r="N2" s="1">
+        <v>56224</v>
+      </c>
+      <c r="O2" s="1">
+        <v>107446</v>
+      </c>
+      <c r="P2" s="1">
+        <v>107446</v>
+      </c>
+      <c r="Q2" s="14">
+        <f>(N2+P2)</f>
+        <v>163670</v>
+      </c>
+    </row>
+    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C3" s="1">
+        <v>47890</v>
+      </c>
+      <c r="D3" s="1">
+        <v>47890</v>
+      </c>
+      <c r="E3" s="1">
+        <v>11327</v>
+      </c>
+      <c r="F3" s="1">
+        <v>11327</v>
+      </c>
+      <c r="G3" s="14">
+        <f t="shared" ref="G3:G4" si="0">(D3+F3)</f>
+        <v>59217</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1008</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1008</v>
+      </c>
+      <c r="J3" s="1">
+        <v>385</v>
+      </c>
+      <c r="K3" s="1">
+        <v>385</v>
+      </c>
+      <c r="L3" s="14">
+        <f t="shared" ref="L3:L4" si="1">(I3+K3)</f>
+        <v>1393</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36644</v>
+      </c>
+      <c r="N3" s="1">
+        <v>36644</v>
+      </c>
+      <c r="O3" s="1">
+        <v>73884</v>
+      </c>
+      <c r="P3" s="1">
+        <v>73884</v>
+      </c>
+      <c r="Q3" s="14">
+        <f t="shared" ref="Q3:Q4" si="2">(N3+P3)</f>
+        <v>110528</v>
+      </c>
+    </row>
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C4" s="1">
+        <v>77800</v>
+      </c>
+      <c r="D4" s="1">
+        <v>77800</v>
+      </c>
+      <c r="E4" s="1">
+        <v>18450</v>
+      </c>
+      <c r="F4" s="1">
+        <v>18450</v>
+      </c>
+      <c r="G4" s="14">
+        <f t="shared" si="0"/>
+        <v>96250</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1714</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1714</v>
+      </c>
+      <c r="J4" s="1">
+        <v>306</v>
+      </c>
+      <c r="K4" s="1">
+        <v>306</v>
+      </c>
+      <c r="L4" s="14">
+        <f t="shared" si="1"/>
+        <v>2020</v>
+      </c>
+      <c r="M4" s="1">
+        <v>50272</v>
+      </c>
+      <c r="N4" s="1">
+        <v>50272</v>
+      </c>
+      <c r="O4" s="1">
+        <v>112428</v>
+      </c>
+      <c r="P4" s="1">
+        <v>112428</v>
+      </c>
+      <c r="Q4" s="14">
+        <f t="shared" si="2"/>
+        <v>162700</v>
+      </c>
+    </row>
+    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C5" s="1">
+        <v>69082</v>
+      </c>
+      <c r="D5" s="14">
+        <f>(D2+D3+D4)/3</f>
+        <v>64206.333333333336</v>
+      </c>
+      <c r="E5" s="1">
+        <v>13920</v>
+      </c>
+      <c r="F5" s="14">
+        <f>(F2+F3+F4)/3</f>
+        <v>17113</v>
+      </c>
+      <c r="G5" s="14">
+        <f>(G2+G3+G4)/3</f>
+        <v>81319.333333333328</v>
+      </c>
+      <c r="H5" s="1">
+        <v>924</v>
+      </c>
+      <c r="I5" s="14">
+        <f>(I2+I3+I4)/3</f>
+        <v>1442.6666666666667</v>
+      </c>
+      <c r="J5" s="1">
+        <v>214</v>
+      </c>
+      <c r="K5" s="14">
+        <f>(K2+K3+K4)/3</f>
+        <v>369.33333333333331</v>
+      </c>
+      <c r="L5" s="14">
+        <f>(L2+L3+L4)/3</f>
+        <v>1812</v>
+      </c>
+      <c r="M5" s="1">
+        <v>37348</v>
+      </c>
+      <c r="N5" s="14">
+        <f>(N2+N3+N4)/3</f>
+        <v>47713.333333333336</v>
+      </c>
+      <c r="O5" s="1">
+        <v>92839</v>
+      </c>
+      <c r="P5" s="14">
+        <f>(P2+P3+P4)/3</f>
+        <v>97919.333333333328</v>
+      </c>
+      <c r="Q5" s="14">
+        <f>(Q2+Q3+Q4)/3</f>
+        <v>145632.66666666666</v>
+      </c>
+    </row>
+    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C6" s="1">
+        <v>237665</v>
+      </c>
+      <c r="D6" s="14">
+        <f t="shared" ref="D6:D37" si="3">(D3+D4+D5)/3</f>
+        <v>63298.777777777781</v>
+      </c>
+      <c r="E6" s="1">
+        <v>120118</v>
+      </c>
+      <c r="F6" s="14">
+        <f t="shared" ref="F6:F37" si="4">(F3+F4+F5)/3</f>
+        <v>15630</v>
+      </c>
+      <c r="G6" s="14">
+        <f t="shared" ref="G6:G37" si="5">(G3+G4+G5)/3</f>
+        <v>78928.777777777766</v>
+      </c>
+      <c r="H6" s="1">
+        <v>8385</v>
+      </c>
+      <c r="I6" s="14">
+        <f t="shared" ref="I6:I37" si="6">(I3+I4+I5)/3</f>
+        <v>1388.2222222222224</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2627</v>
+      </c>
+      <c r="K6" s="14">
+        <f t="shared" ref="K6:K37" si="7">(K3+K4+K5)/3</f>
+        <v>353.4444444444444</v>
+      </c>
+      <c r="L6" s="14">
+        <f t="shared" ref="L6:L37" si="8">(L3+L4+L5)/3</f>
+        <v>1741.6666666666667</v>
+      </c>
+      <c r="M6" s="1">
+        <v>173846</v>
+      </c>
+      <c r="N6" s="14">
+        <f t="shared" ref="N6:N37" si="9">(N3+N4+N5)/3</f>
+        <v>44876.444444444445</v>
+      </c>
+      <c r="O6" s="1">
+        <v>330431</v>
+      </c>
+      <c r="P6" s="14">
+        <f t="shared" ref="P6:P37" si="10">(P3+P4+P5)/3</f>
+        <v>94743.777777777766</v>
+      </c>
+      <c r="Q6" s="14">
+        <f t="shared" ref="Q6:Q37" si="11">(Q3+Q4+Q5)/3</f>
+        <v>139620.22222222222</v>
+      </c>
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C7" s="1">
+        <v>82135</v>
+      </c>
+      <c r="D7" s="14">
+        <f t="shared" si="3"/>
+        <v>68435.037037037036</v>
+      </c>
+      <c r="E7" s="1">
+        <v>19912</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="4"/>
+        <v>17064.333333333332</v>
+      </c>
+      <c r="G7" s="14">
+        <f t="shared" si="5"/>
+        <v>85499.37037037035</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2034</v>
+      </c>
+      <c r="I7" s="14">
+        <f t="shared" si="6"/>
+        <v>1514.9629629629633</v>
+      </c>
+      <c r="J7" s="1">
+        <v>379</v>
+      </c>
+      <c r="K7" s="14">
+        <f t="shared" si="7"/>
+        <v>342.92592592592587</v>
+      </c>
+      <c r="L7" s="14">
+        <f t="shared" si="8"/>
+        <v>1857.8888888888889</v>
+      </c>
+      <c r="M7" s="1">
+        <v>59669</v>
+      </c>
+      <c r="N7" s="14">
+        <f t="shared" si="9"/>
+        <v>47620.592592592591</v>
+      </c>
+      <c r="O7" s="1">
+        <v>125835</v>
+      </c>
+      <c r="P7" s="14">
+        <f t="shared" si="10"/>
+        <v>101697.03703703702</v>
+      </c>
+      <c r="Q7" s="14">
+        <f t="shared" si="11"/>
+        <v>149317.62962962964</v>
+      </c>
+    </row>
+    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C8" s="1">
+        <v>82464</v>
+      </c>
+      <c r="D8" s="14">
+        <f t="shared" si="3"/>
+        <v>65313.382716049382</v>
+      </c>
+      <c r="E8" s="1">
+        <v>16329</v>
+      </c>
+      <c r="F8" s="14">
+        <f t="shared" si="4"/>
+        <v>16602.444444444442</v>
+      </c>
+      <c r="G8" s="14">
+        <f t="shared" si="5"/>
+        <v>81915.82716049382</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1458</v>
+      </c>
+      <c r="I8" s="14">
+        <f t="shared" si="6"/>
+        <v>1448.6172839506173</v>
+      </c>
+      <c r="J8" s="1">
+        <v>279</v>
+      </c>
+      <c r="K8" s="14">
+        <f t="shared" si="7"/>
+        <v>355.23456790123447</v>
+      </c>
+      <c r="L8" s="14">
+        <f t="shared" si="8"/>
+        <v>1803.851851851852</v>
+      </c>
+      <c r="M8" s="1">
+        <v>48428</v>
+      </c>
+      <c r="N8" s="14">
+        <f t="shared" si="9"/>
+        <v>46736.790123456791</v>
+      </c>
+      <c r="O8" s="1">
+        <v>112992</v>
+      </c>
+      <c r="P8" s="14">
+        <f t="shared" si="10"/>
+        <v>98120.049382716024</v>
+      </c>
+      <c r="Q8" s="14">
+        <f t="shared" si="11"/>
+        <v>144856.83950617284</v>
+      </c>
+    </row>
+    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C9" s="1">
+        <v>249792</v>
+      </c>
+      <c r="D9" s="14">
+        <f t="shared" si="3"/>
+        <v>65682.399176954743</v>
+      </c>
+      <c r="E9" s="1">
+        <v>133254</v>
+      </c>
+      <c r="F9" s="14">
+        <f t="shared" si="4"/>
+        <v>16432.259259259259</v>
+      </c>
+      <c r="G9" s="14">
+        <f t="shared" si="5"/>
+        <v>82114.658436213984</v>
+      </c>
+      <c r="H9" s="1">
+        <v>6970</v>
+      </c>
+      <c r="I9" s="14">
+        <f t="shared" si="6"/>
+        <v>1450.6008230452678</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2253</v>
+      </c>
+      <c r="K9" s="14">
+        <f t="shared" si="7"/>
+        <v>350.53497942386821</v>
+      </c>
+      <c r="L9" s="14">
+        <f t="shared" si="8"/>
+        <v>1801.135802469136</v>
+      </c>
+      <c r="M9" s="1">
+        <v>181340</v>
+      </c>
+      <c r="N9" s="14">
+        <f t="shared" si="9"/>
+        <v>46411.275720164609</v>
+      </c>
+      <c r="O9" s="1">
+        <v>346597</v>
+      </c>
+      <c r="P9" s="14">
+        <f t="shared" si="10"/>
+        <v>98186.954732510261</v>
+      </c>
+      <c r="Q9" s="14">
+        <f t="shared" si="11"/>
+        <v>144598.23045267491</v>
+      </c>
+    </row>
+    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C10" s="1">
+        <v>10053</v>
+      </c>
+      <c r="D10" s="14">
+        <f t="shared" si="3"/>
+        <v>66476.939643347054</v>
+      </c>
+      <c r="E10" s="1">
+        <v>4467</v>
+      </c>
+      <c r="F10" s="14">
+        <f t="shared" si="4"/>
+        <v>16699.679012345678</v>
+      </c>
+      <c r="G10" s="14">
+        <f t="shared" si="5"/>
+        <v>83176.618655692713</v>
+      </c>
+      <c r="H10" s="1">
+        <v>233</v>
+      </c>
+      <c r="I10" s="14">
+        <f t="shared" si="6"/>
+        <v>1471.3936899862829</v>
+      </c>
+      <c r="J10" s="1">
+        <v>163</v>
+      </c>
+      <c r="K10" s="14">
+        <f t="shared" si="7"/>
+        <v>349.56515775034285</v>
+      </c>
+      <c r="L10" s="14">
+        <f t="shared" si="8"/>
+        <v>1820.9588477366258</v>
+      </c>
+      <c r="M10" s="1">
+        <v>10647</v>
+      </c>
+      <c r="N10" s="14">
+        <f t="shared" si="9"/>
+        <v>46922.886145404664</v>
+      </c>
+      <c r="O10" s="1">
+        <v>17246</v>
+      </c>
+      <c r="P10" s="14">
+        <f t="shared" si="10"/>
+        <v>99334.680384087769</v>
+      </c>
+      <c r="Q10" s="14">
+        <f t="shared" si="11"/>
+        <v>146257.56652949247</v>
+      </c>
+    </row>
+    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C11" s="1">
+        <v>42869</v>
+      </c>
+      <c r="D11" s="14">
+        <f t="shared" si="3"/>
+        <v>65824.24051211706</v>
+      </c>
+      <c r="E11" s="1">
+        <v>8135</v>
+      </c>
+      <c r="F11" s="14">
+        <f t="shared" si="4"/>
+        <v>16578.127572016459</v>
+      </c>
+      <c r="G11" s="14">
+        <f t="shared" si="5"/>
+        <v>82402.368084133501</v>
+      </c>
+      <c r="H11" s="1">
+        <v>369</v>
+      </c>
+      <c r="I11" s="14">
+        <f t="shared" si="6"/>
+        <v>1456.8705989940561</v>
+      </c>
+      <c r="J11" s="1">
+        <v>79</v>
+      </c>
+      <c r="K11" s="14">
+        <f t="shared" si="7"/>
+        <v>351.77823502514849</v>
+      </c>
+      <c r="L11" s="14">
+        <f t="shared" si="8"/>
+        <v>1808.6488340192045</v>
+      </c>
+      <c r="M11" s="1">
+        <v>22965</v>
+      </c>
+      <c r="N11" s="14">
+        <f t="shared" si="9"/>
+        <v>46690.317329675359</v>
+      </c>
+      <c r="O11" s="1">
+        <v>59150</v>
+      </c>
+      <c r="P11" s="14">
+        <f t="shared" si="10"/>
+        <v>98547.228166438013</v>
+      </c>
+      <c r="Q11" s="14">
+        <f t="shared" si="11"/>
+        <v>145237.54549611339</v>
+      </c>
+    </row>
+    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C12" s="1">
+        <v>6466</v>
+      </c>
+      <c r="D12" s="14">
+        <f t="shared" si="3"/>
+        <v>65994.526444139614</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2809</v>
+      </c>
+      <c r="F12" s="14">
+        <f t="shared" si="4"/>
+        <v>16570.0219478738</v>
+      </c>
+      <c r="G12" s="14">
+        <f t="shared" si="5"/>
+        <v>82564.548392013399</v>
+      </c>
+      <c r="H12" s="1">
+        <v>280</v>
+      </c>
+      <c r="I12" s="14">
+        <f t="shared" si="6"/>
+        <v>1459.6217040085357</v>
+      </c>
+      <c r="J12" s="1">
+        <v>66</v>
+      </c>
+      <c r="K12" s="14">
+        <f t="shared" si="7"/>
+        <v>350.6261240664532</v>
+      </c>
+      <c r="L12" s="14">
+        <f t="shared" si="8"/>
+        <v>1810.2478280749885</v>
+      </c>
+      <c r="M12" s="1">
+        <v>5551</v>
+      </c>
+      <c r="N12" s="14">
+        <f t="shared" si="9"/>
+        <v>46674.82639841488</v>
+      </c>
+      <c r="O12" s="1">
+        <v>10065</v>
+      </c>
+      <c r="P12" s="14">
+        <f t="shared" si="10"/>
+        <v>98689.621094345348</v>
+      </c>
+      <c r="Q12" s="14">
+        <f t="shared" si="11"/>
+        <v>145364.44749276026</v>
+      </c>
+    </row>
+    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C13" s="1">
+        <v>34039</v>
+      </c>
+      <c r="D13" s="14">
+        <f t="shared" si="3"/>
+        <v>66098.568866534566</v>
+      </c>
+      <c r="E13" s="1">
+        <v>7573</v>
+      </c>
+      <c r="F13" s="14">
+        <f t="shared" si="4"/>
+        <v>16615.942844078647</v>
+      </c>
+      <c r="G13" s="14">
+        <f t="shared" si="5"/>
+        <v>82714.511710613209</v>
+      </c>
+      <c r="H13" s="1">
+        <v>465</v>
+      </c>
+      <c r="I13" s="14">
+        <f t="shared" si="6"/>
+        <v>1462.6286643296251</v>
+      </c>
+      <c r="J13" s="1">
+        <v>94</v>
+      </c>
+      <c r="K13" s="14">
+        <f t="shared" si="7"/>
+        <v>350.65650561398155</v>
+      </c>
+      <c r="L13" s="14">
+        <f t="shared" si="8"/>
+        <v>1813.2851699436062</v>
+      </c>
+      <c r="M13" s="1">
+        <v>21586</v>
+      </c>
+      <c r="N13" s="14">
+        <f t="shared" si="9"/>
+        <v>46762.676624498301</v>
+      </c>
+      <c r="O13" s="1">
+        <v>51174</v>
+      </c>
+      <c r="P13" s="14">
+        <f t="shared" si="10"/>
+        <v>98857.176548290372</v>
+      </c>
+      <c r="Q13" s="14">
+        <f t="shared" si="11"/>
+        <v>145619.85317278872</v>
+      </c>
+    </row>
+    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C14" s="1">
+        <v>66461</v>
+      </c>
+      <c r="D14" s="14">
+        <f t="shared" si="3"/>
+        <v>65972.445274263751</v>
+      </c>
+      <c r="E14" s="1">
+        <v>7671</v>
+      </c>
+      <c r="F14" s="14">
+        <f t="shared" si="4"/>
+        <v>16588.030787989632</v>
+      </c>
+      <c r="G14" s="14">
+        <f t="shared" si="5"/>
+        <v>82560.476062253365</v>
+      </c>
+      <c r="H14" s="1">
+        <v>463</v>
+      </c>
+      <c r="I14" s="14">
+        <f t="shared" si="6"/>
+        <v>1459.7069891107392</v>
+      </c>
+      <c r="J14" s="1">
+        <v>71</v>
+      </c>
+      <c r="K14" s="14">
+        <f t="shared" si="7"/>
+        <v>351.02028823519441</v>
+      </c>
+      <c r="L14" s="14">
+        <f t="shared" si="8"/>
+        <v>1810.7272773459329</v>
+      </c>
+      <c r="M14" s="1">
+        <v>27669</v>
+      </c>
+      <c r="N14" s="14">
+        <f t="shared" si="9"/>
+        <v>46709.273450862849</v>
+      </c>
+      <c r="O14" s="1">
+        <v>83130</v>
+      </c>
+      <c r="P14" s="14">
+        <f t="shared" si="10"/>
+        <v>98698.008603024573</v>
+      </c>
+      <c r="Q14" s="14">
+        <f t="shared" si="11"/>
+        <v>145407.28205388747</v>
+      </c>
+    </row>
+    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
+        <v>27861</v>
+      </c>
+      <c r="D15" s="14">
+        <f t="shared" si="3"/>
+        <v>66021.846861645972</v>
+      </c>
+      <c r="E15" s="1">
+        <v>4606</v>
+      </c>
+      <c r="F15" s="14">
+        <f t="shared" si="4"/>
+        <v>16591.331859980692</v>
+      </c>
+      <c r="G15" s="14">
+        <f t="shared" si="5"/>
+        <v>82613.178721626653</v>
+      </c>
+      <c r="H15" s="1">
+        <v>169</v>
+      </c>
+      <c r="I15" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.6524524829667</v>
+      </c>
+      <c r="J15" s="1">
+        <v>52</v>
+      </c>
+      <c r="K15" s="14">
+        <f t="shared" si="7"/>
+        <v>350.76763930520974</v>
+      </c>
+      <c r="L15" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.420091788176</v>
+      </c>
+      <c r="M15" s="1">
+        <v>12251</v>
+      </c>
+      <c r="N15" s="14">
+        <f t="shared" si="9"/>
+        <v>46715.592157925341</v>
+      </c>
+      <c r="O15" s="1">
+        <v>35725</v>
+      </c>
+      <c r="P15" s="14">
+        <f t="shared" si="10"/>
+        <v>98748.268748553426</v>
+      </c>
+      <c r="Q15" s="14">
+        <f t="shared" si="11"/>
+        <v>145463.86090647883</v>
+      </c>
+    </row>
+    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C16" s="1">
+        <v>92941</v>
+      </c>
+      <c r="D16" s="14">
+        <f t="shared" si="3"/>
+        <v>66030.95366748143</v>
+      </c>
+      <c r="E16" s="1">
+        <v>15311</v>
+      </c>
+      <c r="F16" s="14">
+        <f t="shared" si="4"/>
+        <v>16598.435164016322</v>
+      </c>
+      <c r="G16" s="14">
+        <f t="shared" si="5"/>
+        <v>82629.388831497738</v>
+      </c>
+      <c r="H16" s="1">
+        <v>862</v>
+      </c>
+      <c r="I16" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.996035307777</v>
+      </c>
+      <c r="J16" s="1">
+        <v>238</v>
+      </c>
+      <c r="K16" s="14">
+        <f t="shared" si="7"/>
+        <v>350.8148110514619</v>
+      </c>
+      <c r="L16" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.8108463592382</v>
+      </c>
+      <c r="M16" s="1">
+        <v>56667</v>
+      </c>
+      <c r="N16" s="14">
+        <f t="shared" si="9"/>
+        <v>46729.180744428828</v>
+      </c>
+      <c r="O16" s="1">
+        <v>133718</v>
+      </c>
+      <c r="P16" s="14">
+        <f t="shared" si="10"/>
+        <v>98767.817966622781</v>
+      </c>
+      <c r="Q16" s="14">
+        <f t="shared" si="11"/>
+        <v>145496.99871105168</v>
+      </c>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>78861</v>
+      </c>
+      <c r="D17" s="14">
+        <f t="shared" si="3"/>
+        <v>66008.415267797056</v>
+      </c>
+      <c r="E17" s="1">
+        <v>13827</v>
+      </c>
+      <c r="F17" s="14">
+        <f t="shared" si="4"/>
+        <v>16592.599270662216</v>
+      </c>
+      <c r="G17" s="14">
+        <f t="shared" si="5"/>
+        <v>82601.014538459247</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1580</v>
+      </c>
+      <c r="I17" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.4518256338276</v>
+      </c>
+      <c r="J17" s="1">
+        <v>287</v>
+      </c>
+      <c r="K17" s="14">
+        <f t="shared" si="7"/>
+        <v>350.86757953062198</v>
+      </c>
+      <c r="L17" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.3194051644489</v>
+      </c>
+      <c r="M17" s="1">
+        <v>54441</v>
+      </c>
+      <c r="N17" s="14">
+        <f t="shared" si="9"/>
+        <v>46718.015451072337</v>
+      </c>
+      <c r="O17" s="1">
+        <v>110055</v>
+      </c>
+      <c r="P17" s="14">
+        <f t="shared" si="10"/>
+        <v>98738.031772733593</v>
+      </c>
+      <c r="Q17" s="14">
+        <f t="shared" si="11"/>
+        <v>145456.047223806</v>
+      </c>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <v>29519</v>
+      </c>
+      <c r="D18" s="14">
+        <f t="shared" si="3"/>
+        <v>66020.405265641501</v>
+      </c>
+      <c r="E18" s="1">
+        <v>6647</v>
+      </c>
+      <c r="F18" s="14">
+        <f t="shared" si="4"/>
+        <v>16594.122098219745</v>
+      </c>
+      <c r="G18" s="14">
+        <f t="shared" si="5"/>
+        <v>82614.527363861213</v>
+      </c>
+      <c r="H18" s="1">
+        <v>605</v>
+      </c>
+      <c r="I18" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.700104474857</v>
+      </c>
+      <c r="J18" s="1">
+        <v>74</v>
+      </c>
+      <c r="K18" s="14">
+        <f t="shared" si="7"/>
+        <v>350.81667662909786</v>
+      </c>
+      <c r="L18" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.5167811039544</v>
+      </c>
+      <c r="M18" s="1">
+        <v>25598</v>
+      </c>
+      <c r="N18" s="14">
+        <f t="shared" si="9"/>
+        <v>46720.929451142169</v>
+      </c>
+      <c r="O18" s="1">
+        <v>51851</v>
+      </c>
+      <c r="P18" s="14">
+        <f t="shared" si="10"/>
+        <v>98751.372829303262</v>
+      </c>
+      <c r="Q18" s="14">
+        <f t="shared" si="11"/>
+        <v>145472.3022804455</v>
+      </c>
+    </row>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <v>93908</v>
+      </c>
+      <c r="D19" s="14">
+        <f t="shared" si="3"/>
+        <v>66019.92473364</v>
+      </c>
+      <c r="E19" s="1">
+        <v>24116</v>
+      </c>
+      <c r="F19" s="14">
+        <f t="shared" si="4"/>
+        <v>16595.052177632762</v>
+      </c>
+      <c r="G19" s="14">
+        <f t="shared" si="5"/>
+        <v>82614.976911272737</v>
+      </c>
+      <c r="H19" s="1">
+        <v>2049</v>
+      </c>
+      <c r="I19" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.7159884721539</v>
+      </c>
+      <c r="J19" s="1">
+        <v>508</v>
+      </c>
+      <c r="K19" s="14">
+        <f t="shared" si="7"/>
+        <v>350.83302240372723</v>
+      </c>
+      <c r="L19" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.5490108758804</v>
+      </c>
+      <c r="M19" s="1">
+        <v>75497</v>
+      </c>
+      <c r="N19" s="14">
+        <f t="shared" si="9"/>
+        <v>46722.708548881114</v>
+      </c>
+      <c r="O19" s="1">
+        <v>151272</v>
+      </c>
+      <c r="P19" s="14">
+        <f t="shared" si="10"/>
+        <v>98752.40752288654</v>
+      </c>
+      <c r="Q19" s="14">
+        <f t="shared" si="11"/>
+        <v>145475.11607176773</v>
+      </c>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C20" s="1">
+        <v>91427</v>
+      </c>
+      <c r="D20" s="14">
+        <f t="shared" si="3"/>
+        <v>66016.248422359524</v>
+      </c>
+      <c r="E20" s="1">
+        <v>32543</v>
+      </c>
+      <c r="F20" s="14">
+        <f t="shared" si="4"/>
+        <v>16593.92451550491</v>
+      </c>
+      <c r="G20" s="14">
+        <f t="shared" si="5"/>
+        <v>82610.172937864394</v>
+      </c>
+      <c r="H20" s="1">
+        <v>2742</v>
+      </c>
+      <c r="I20" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.6226395269462</v>
+      </c>
+      <c r="J20" s="1">
+        <v>977</v>
+      </c>
+      <c r="K20" s="14">
+        <f t="shared" si="7"/>
+        <v>350.83909285448232</v>
+      </c>
+      <c r="L20" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.461732381428</v>
+      </c>
+      <c r="M20" s="1">
+        <v>90812</v>
+      </c>
+      <c r="N20" s="14">
+        <f t="shared" si="9"/>
+        <v>46720.551150365209</v>
+      </c>
+      <c r="O20" s="1">
+        <v>166663</v>
+      </c>
+      <c r="P20" s="14">
+        <f t="shared" si="10"/>
+        <v>98747.270708307798</v>
+      </c>
+      <c r="Q20" s="14">
+        <f t="shared" si="11"/>
+        <v>145467.82185867309</v>
+      </c>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C21" s="1">
+        <v>67751</v>
+      </c>
+      <c r="D21" s="14">
+        <f t="shared" si="3"/>
+        <v>66018.859473880337</v>
+      </c>
+      <c r="E21" s="1">
+        <v>18401</v>
+      </c>
+      <c r="F21" s="14">
+        <f t="shared" si="4"/>
+        <v>16594.366263785807</v>
+      </c>
+      <c r="G21" s="14">
+        <f t="shared" si="5"/>
+        <v>82613.225737666115</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1549</v>
+      </c>
+      <c r="I21" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.6795774913189</v>
+      </c>
+      <c r="J21" s="1">
+        <v>347</v>
+      </c>
+      <c r="K21" s="14">
+        <f t="shared" si="7"/>
+        <v>350.82959729576913</v>
+      </c>
+      <c r="L21" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.5091747870877</v>
+      </c>
+      <c r="M21" s="1">
+        <v>62082</v>
+      </c>
+      <c r="N21" s="14">
+        <f t="shared" si="9"/>
+        <v>46721.39638346283</v>
+      </c>
+      <c r="O21" s="1">
+        <v>119503</v>
+      </c>
+      <c r="P21" s="14">
+        <f t="shared" si="10"/>
+        <v>98750.350353499191</v>
+      </c>
+      <c r="Q21" s="14">
+        <f t="shared" si="11"/>
+        <v>145471.74673696212</v>
+      </c>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C22" s="1">
+        <v>117055</v>
+      </c>
+      <c r="D22" s="14">
+        <f t="shared" si="3"/>
+        <v>66018.344209959949</v>
+      </c>
+      <c r="E22" s="1">
+        <v>32245</v>
+      </c>
+      <c r="F22" s="14">
+        <f t="shared" si="4"/>
+        <v>16594.447652307827</v>
+      </c>
+      <c r="G22" s="14">
+        <f t="shared" si="5"/>
+        <v>82612.791862267753</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1979</v>
+      </c>
+      <c r="I22" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.6727351634729</v>
+      </c>
+      <c r="J22" s="1">
+        <v>477</v>
+      </c>
+      <c r="K22" s="14">
+        <f t="shared" si="7"/>
+        <v>350.83390418465956</v>
+      </c>
+      <c r="L22" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.506639348132</v>
+      </c>
+      <c r="M22" s="1">
+        <v>90231</v>
+      </c>
+      <c r="N22" s="14">
+        <f t="shared" si="9"/>
+        <v>46721.552027569713</v>
+      </c>
+      <c r="O22" s="1">
+        <v>189094</v>
+      </c>
+      <c r="P22" s="14">
+        <f t="shared" si="10"/>
+        <v>98750.009528231167</v>
+      </c>
+      <c r="Q22" s="14">
+        <f t="shared" si="11"/>
+        <v>145471.56155580099</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C23" s="1">
+        <v>95661</v>
+      </c>
+      <c r="D23" s="14">
+        <f t="shared" si="3"/>
+        <v>66017.817368733275</v>
+      </c>
+      <c r="E23" s="1">
+        <v>23423</v>
+      </c>
+      <c r="F23" s="14">
+        <f t="shared" si="4"/>
+        <v>16594.246143866181</v>
+      </c>
+      <c r="G23" s="14">
+        <f t="shared" si="5"/>
+        <v>82612.06351259943</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1336</v>
+      </c>
+      <c r="I23" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.6583173939125</v>
+      </c>
+      <c r="J23" s="1">
+        <v>316</v>
+      </c>
+      <c r="K23" s="14">
+        <f t="shared" si="7"/>
+        <v>350.83419811163702</v>
+      </c>
+      <c r="L23" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.4925155055491</v>
+      </c>
+      <c r="M23" s="1">
+        <v>62784</v>
+      </c>
+      <c r="N23" s="14">
+        <f t="shared" si="9"/>
+        <v>46721.166520465915</v>
+      </c>
+      <c r="O23" s="1">
+        <v>141119</v>
+      </c>
+      <c r="P23" s="14">
+        <f t="shared" si="10"/>
+        <v>98749.210196679385</v>
+      </c>
+      <c r="Q23" s="14">
+        <f t="shared" si="11"/>
+        <v>145470.37671714541</v>
+      </c>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C24" s="1">
+        <v>339512</v>
+      </c>
+      <c r="D24" s="14">
+        <f t="shared" si="3"/>
+        <v>66018.340350857863</v>
+      </c>
+      <c r="E24" s="1">
+        <v>168442</v>
+      </c>
+      <c r="F24" s="14">
+        <f t="shared" si="4"/>
+        <v>16594.353353319937</v>
+      </c>
+      <c r="G24" s="14">
+        <f t="shared" si="5"/>
+        <v>82612.693704177756</v>
+      </c>
+      <c r="H24" s="1">
+        <v>11651</v>
+      </c>
+      <c r="I24" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.6702100162347</v>
+      </c>
+      <c r="J24" s="1">
+        <v>4407</v>
+      </c>
+      <c r="K24" s="14">
+        <f t="shared" si="7"/>
+        <v>350.83256653068861</v>
+      </c>
+      <c r="L24" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.5027765469229</v>
+      </c>
+      <c r="M24" s="1">
+        <v>309483</v>
+      </c>
+      <c r="N24" s="14">
+        <f t="shared" si="9"/>
+        <v>46721.371643832819</v>
+      </c>
+      <c r="O24" s="1">
+        <v>551686</v>
+      </c>
+      <c r="P24" s="14">
+        <f t="shared" si="10"/>
+        <v>98749.856692803252</v>
+      </c>
+      <c r="Q24" s="14">
+        <f t="shared" si="11"/>
+        <v>145471.22833663618</v>
+      </c>
+    </row>
+    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C25" s="1">
+        <v>99759</v>
+      </c>
+      <c r="D25" s="14">
+        <f t="shared" si="3"/>
+        <v>66018.167309850352</v>
+      </c>
+      <c r="E25" s="1">
+        <v>24192</v>
+      </c>
+      <c r="F25" s="14">
+        <f t="shared" si="4"/>
+        <v>16594.349049831315</v>
+      </c>
+      <c r="G25" s="14">
+        <f t="shared" si="5"/>
+        <v>82612.516359681656</v>
+      </c>
+      <c r="H25" s="1">
+        <v>2406</v>
+      </c>
+      <c r="I25" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.66708752454</v>
+      </c>
+      <c r="J25" s="1">
+        <v>609</v>
+      </c>
+      <c r="K25" s="14">
+        <f t="shared" si="7"/>
+        <v>350.83355627566175</v>
+      </c>
+      <c r="L25" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.5006438002013</v>
+      </c>
+      <c r="M25" s="1">
+        <v>90038</v>
+      </c>
+      <c r="N25" s="14">
+        <f t="shared" si="9"/>
+        <v>46721.363397289482</v>
+      </c>
+      <c r="O25" s="1">
+        <v>173420</v>
+      </c>
+      <c r="P25" s="14">
+        <f t="shared" si="10"/>
+        <v>98749.692139237945</v>
+      </c>
+      <c r="Q25" s="14">
+        <f t="shared" si="11"/>
+        <v>145471.05553652754</v>
+      </c>
+    </row>
+    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C26" s="1">
+        <v>117668</v>
+      </c>
+      <c r="D26" s="14">
+        <f t="shared" si="3"/>
+        <v>66018.108343147163</v>
+      </c>
+      <c r="E26" s="1">
+        <v>23670</v>
+      </c>
+      <c r="F26" s="14">
+        <f t="shared" si="4"/>
+        <v>16594.316182339146</v>
+      </c>
+      <c r="G26" s="14">
+        <f t="shared" si="5"/>
+        <v>82612.424525486291</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1643</v>
+      </c>
+      <c r="I26" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.665204978229</v>
+      </c>
+      <c r="J26" s="1">
+        <v>466</v>
+      </c>
+      <c r="K26" s="14">
+        <f t="shared" si="7"/>
+        <v>350.83344030599579</v>
+      </c>
+      <c r="L26" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.4986452842243</v>
+      </c>
+      <c r="M26" s="1">
+        <v>78265</v>
+      </c>
+      <c r="N26" s="14">
+        <f t="shared" si="9"/>
+        <v>46721.30052052941</v>
+      </c>
+      <c r="O26" s="1">
+        <v>171853</v>
+      </c>
+      <c r="P26" s="14">
+        <f t="shared" si="10"/>
+        <v>98749.586342906856</v>
+      </c>
+      <c r="Q26" s="14">
+        <f t="shared" si="11"/>
+        <v>145470.88686343638</v>
+      </c>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C27" s="1">
+        <v>336106</v>
+      </c>
+      <c r="D27" s="14">
+        <f t="shared" si="3"/>
+        <v>66018.205334618455</v>
+      </c>
+      <c r="E27" s="1">
+        <v>184065</v>
+      </c>
+      <c r="F27" s="14">
+        <f t="shared" si="4"/>
+        <v>16594.339528496799</v>
+      </c>
+      <c r="G27" s="14">
+        <f t="shared" si="5"/>
+        <v>82612.544863115239</v>
+      </c>
+      <c r="H27" s="1">
+        <v>11948</v>
+      </c>
+      <c r="I27" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.6675008396678</v>
+      </c>
+      <c r="J27" s="1">
+        <v>5001</v>
+      </c>
+      <c r="K27" s="14">
+        <f t="shared" si="7"/>
+        <v>350.83318770411535</v>
+      </c>
+      <c r="L27" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.5006885437826</v>
+      </c>
+      <c r="M27" s="1">
+        <v>291134</v>
+      </c>
+      <c r="N27" s="14">
+        <f t="shared" si="9"/>
+        <v>46721.345187217237</v>
+      </c>
+      <c r="O27" s="1">
+        <v>523332</v>
+      </c>
+      <c r="P27" s="14">
+        <f t="shared" si="10"/>
+        <v>98749.711724982699</v>
+      </c>
+      <c r="Q27" s="14">
+        <f t="shared" si="11"/>
+        <v>145471.05691220003</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C28" s="1">
+        <v>14321</v>
+      </c>
+      <c r="D28" s="14">
+        <f t="shared" si="3"/>
+        <v>66018.160329205319</v>
+      </c>
+      <c r="E28" s="1">
+        <v>7894</v>
+      </c>
+      <c r="F28" s="14">
+        <f t="shared" si="4"/>
+        <v>16594.33492022242</v>
+      </c>
+      <c r="G28" s="14">
+        <f t="shared" si="5"/>
+        <v>82612.495249427724</v>
+      </c>
+      <c r="H28" s="1">
+        <v>819</v>
+      </c>
+      <c r="I28" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.6665977808123</v>
+      </c>
+      <c r="J28" s="1">
+        <v>510</v>
+      </c>
+      <c r="K28" s="14">
+        <f t="shared" si="7"/>
+        <v>350.83339476192424</v>
+      </c>
+      <c r="L28" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.4999925427362</v>
+      </c>
+      <c r="M28" s="1">
+        <v>23092</v>
+      </c>
+      <c r="N28" s="14">
+        <f t="shared" si="9"/>
+        <v>46721.336368345372</v>
+      </c>
+      <c r="O28" s="1">
+        <v>31869</v>
+      </c>
+      <c r="P28" s="14">
+        <f t="shared" si="10"/>
+        <v>98749.663402375838</v>
+      </c>
+      <c r="Q28" s="14">
+        <f t="shared" si="11"/>
+        <v>145470.9997707213</v>
+      </c>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C29" s="1">
+        <v>59713</v>
+      </c>
+      <c r="D29" s="14">
+        <f t="shared" si="3"/>
+        <v>66018.158002323646</v>
+      </c>
+      <c r="E29" s="1">
+        <v>13802</v>
+      </c>
+      <c r="F29" s="14">
+        <f t="shared" si="4"/>
+        <v>16594.330210352786</v>
+      </c>
+      <c r="G29" s="14">
+        <f t="shared" si="5"/>
+        <v>82612.488212676428</v>
+      </c>
+      <c r="H29" s="1">
+        <v>473</v>
+      </c>
+      <c r="I29" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.6664345329029</v>
+      </c>
+      <c r="J29" s="1">
+        <v>123</v>
+      </c>
+      <c r="K29" s="14">
+        <f t="shared" si="7"/>
+        <v>350.83334092401179</v>
+      </c>
+      <c r="L29" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.4997754569142</v>
+      </c>
+      <c r="M29" s="1">
+        <v>38880</v>
+      </c>
+      <c r="N29" s="14">
+        <f t="shared" si="9"/>
+        <v>46721.327358697337</v>
+      </c>
+      <c r="O29" s="1">
+        <v>90523</v>
+      </c>
+      <c r="P29" s="14">
+        <f t="shared" si="10"/>
+        <v>98749.653823421802</v>
+      </c>
+      <c r="Q29" s="14">
+        <f t="shared" si="11"/>
+        <v>145470.98118211923</v>
+      </c>
+    </row>
+    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C30" s="1">
+        <v>13463</v>
+      </c>
+      <c r="D30" s="14">
+        <f t="shared" si="3"/>
+        <v>66018.174555382473</v>
+      </c>
+      <c r="E30" s="1">
+        <v>6941</v>
+      </c>
+      <c r="F30" s="14">
+        <f t="shared" si="4"/>
+        <v>16594.334886357334</v>
+      </c>
+      <c r="G30" s="14">
+        <f t="shared" si="5"/>
+        <v>82612.509441739807</v>
+      </c>
+      <c r="H30" s="1">
+        <v>480</v>
+      </c>
+      <c r="I30" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.666844384461</v>
+      </c>
+      <c r="J30" s="1">
+        <v>216</v>
+      </c>
+      <c r="K30" s="14">
+        <f t="shared" si="7"/>
+        <v>350.83330779668381</v>
+      </c>
+      <c r="L30" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.5001521811444</v>
+      </c>
+      <c r="M30" s="1">
+        <v>12583</v>
+      </c>
+      <c r="N30" s="14">
+        <f t="shared" si="9"/>
+        <v>46721.33630475332</v>
+      </c>
+      <c r="O30" s="1">
+        <v>20824</v>
+      </c>
+      <c r="P30" s="14">
+        <f t="shared" si="10"/>
+        <v>98749.67631692678</v>
+      </c>
+      <c r="Q30" s="14">
+        <f t="shared" si="11"/>
+        <v>145471.01262168019</v>
+      </c>
+    </row>
+    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C31" s="1">
+        <v>48168</v>
+      </c>
+      <c r="D31" s="14">
+        <f t="shared" si="3"/>
+        <v>66018.164295637151</v>
+      </c>
+      <c r="E31" s="1">
+        <v>11848</v>
+      </c>
+      <c r="F31" s="14">
+        <f t="shared" si="4"/>
+        <v>16594.333338977511</v>
+      </c>
+      <c r="G31" s="14">
+        <f t="shared" si="5"/>
+        <v>82612.497634614658</v>
+      </c>
+      <c r="H31" s="1">
+        <v>626</v>
+      </c>
+      <c r="I31" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.6666255660587</v>
+      </c>
+      <c r="J31" s="1">
+        <v>103</v>
+      </c>
+      <c r="K31" s="14">
+        <f t="shared" si="7"/>
+        <v>350.83334782753991</v>
+      </c>
+      <c r="L31" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.4999733935983</v>
+      </c>
+      <c r="M31" s="1">
+        <v>35422</v>
+      </c>
+      <c r="N31" s="14">
+        <f t="shared" si="9"/>
+        <v>46721.333343932005</v>
+      </c>
+      <c r="O31" s="1">
+        <v>77484</v>
+      </c>
+      <c r="P31" s="14">
+        <f t="shared" si="10"/>
+        <v>98749.664514241464</v>
+      </c>
+      <c r="Q31" s="14">
+        <f t="shared" si="11"/>
+        <v>145470.99785817356</v>
+      </c>
+    </row>
+    <row r="32" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C32" s="1">
+        <v>83156</v>
+      </c>
+      <c r="D32" s="14">
+        <f t="shared" si="3"/>
+        <v>66018.165617781095</v>
+      </c>
+      <c r="E32" s="1">
+        <v>9842</v>
+      </c>
+      <c r="F32" s="14">
+        <f t="shared" si="4"/>
+        <v>16594.332811895874</v>
+      </c>
+      <c r="G32" s="14">
+        <f t="shared" si="5"/>
+        <v>82612.498429676969</v>
+      </c>
+      <c r="H32" s="1">
+        <v>588</v>
+      </c>
+      <c r="I32" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.6666348278075</v>
+      </c>
+      <c r="J32" s="1">
+        <v>121</v>
+      </c>
+      <c r="K32" s="14">
+        <f t="shared" si="7"/>
+        <v>350.83333218274515</v>
+      </c>
+      <c r="L32" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.4999670105524</v>
+      </c>
+      <c r="M32" s="1">
+        <v>55966</v>
+      </c>
+      <c r="N32" s="14">
+        <f t="shared" si="9"/>
+        <v>46721.332335794221</v>
+      </c>
+      <c r="O32" s="1">
+        <v>129482</v>
+      </c>
+      <c r="P32" s="14">
+        <f t="shared" si="10"/>
+        <v>98749.664884863349</v>
+      </c>
+      <c r="Q32" s="14">
+        <f t="shared" si="11"/>
+        <v>145470.99722065765</v>
+      </c>
+    </row>
+    <row r="33" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C33" s="1">
+        <v>41242</v>
+      </c>
+      <c r="D33" s="14">
+        <f t="shared" si="3"/>
+        <v>66018.168156266911</v>
+      </c>
+      <c r="E33" s="1">
+        <v>8277</v>
+      </c>
+      <c r="F33" s="14">
+        <f t="shared" si="4"/>
+        <v>16594.333679076906</v>
+      </c>
+      <c r="G33" s="14">
+        <f t="shared" si="5"/>
+        <v>82612.501835343821</v>
+      </c>
+      <c r="H33" s="1">
+        <v>385</v>
+      </c>
+      <c r="I33" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.6667015927758</v>
+      </c>
+      <c r="J33" s="1">
+        <v>101</v>
+      </c>
+      <c r="K33" s="14">
+        <f t="shared" si="7"/>
+        <v>350.83332926898964</v>
+      </c>
+      <c r="L33" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.5000308617653</v>
+      </c>
+      <c r="M33" s="1">
+        <v>21834</v>
+      </c>
+      <c r="N33" s="14">
+        <f t="shared" si="9"/>
+        <v>46721.333994826513</v>
+      </c>
+      <c r="O33" s="1">
+        <v>57077</v>
+      </c>
+      <c r="P33" s="14">
+        <f t="shared" si="10"/>
+        <v>98749.668572010531</v>
+      </c>
+      <c r="Q33" s="14">
+        <f t="shared" si="11"/>
+        <v>145471.00256683712</v>
+      </c>
+    </row>
+    <row r="34" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C34" s="1">
+        <v>123320</v>
+      </c>
+      <c r="D34" s="14">
+        <f t="shared" si="3"/>
+        <v>66018.16602322839</v>
+      </c>
+      <c r="E34" s="1">
+        <v>25939</v>
+      </c>
+      <c r="F34" s="14">
+        <f t="shared" si="4"/>
+        <v>16594.333276650097</v>
+      </c>
+      <c r="G34" s="14">
+        <f t="shared" si="5"/>
+        <v>82612.499299878487</v>
+      </c>
+      <c r="H34" s="1">
+        <v>1734</v>
+      </c>
+      <c r="I34" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.6666539955474</v>
+      </c>
+      <c r="J34" s="1">
+        <v>482</v>
+      </c>
+      <c r="K34" s="14">
+        <f t="shared" si="7"/>
+        <v>350.83333642642492</v>
+      </c>
+      <c r="L34" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.4999904219721</v>
+      </c>
+      <c r="M34" s="1">
+        <v>99334</v>
+      </c>
+      <c r="N34" s="14">
+        <f t="shared" si="9"/>
+        <v>46721.33322485091</v>
+      </c>
+      <c r="O34" s="1">
+        <v>204578</v>
+      </c>
+      <c r="P34" s="14">
+        <f t="shared" si="10"/>
+        <v>98749.665990371781</v>
+      </c>
+      <c r="Q34" s="14">
+        <f t="shared" si="11"/>
+        <v>145470.99921522278</v>
+      </c>
+    </row>
+    <row r="35" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C35" s="1">
+        <v>107163</v>
+      </c>
+      <c r="D35" s="14">
+        <f t="shared" si="3"/>
+        <v>66018.166599092132</v>
+      </c>
+      <c r="E35" s="1">
+        <v>19326</v>
+      </c>
+      <c r="F35" s="14">
+        <f t="shared" si="4"/>
+        <v>16594.333255874295</v>
+      </c>
+      <c r="G35" s="14">
+        <f t="shared" si="5"/>
+        <v>82612.499854966431</v>
+      </c>
+      <c r="H35" s="1">
+        <v>1651</v>
+      </c>
+      <c r="I35" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.6666634720434</v>
+      </c>
+      <c r="J35" s="1">
+        <v>317</v>
+      </c>
+      <c r="K35" s="14">
+        <f t="shared" si="7"/>
+        <v>350.83333262605328</v>
+      </c>
+      <c r="L35" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.4999960980967</v>
+      </c>
+      <c r="M35" s="1">
+        <v>79698</v>
+      </c>
+      <c r="N35" s="14">
+        <f t="shared" si="9"/>
+        <v>46721.333185157215</v>
+      </c>
+      <c r="O35" s="1">
+        <v>163224</v>
+      </c>
+      <c r="P35" s="14">
+        <f t="shared" si="10"/>
+        <v>98749.666482415225</v>
+      </c>
+      <c r="Q35" s="14">
+        <f t="shared" si="11"/>
+        <v>145470.99966757253</v>
+      </c>
+    </row>
+    <row r="36" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C36" s="1">
+        <v>39652</v>
+      </c>
+      <c r="D36" s="14">
+        <f t="shared" si="3"/>
+        <v>66018.166926195801</v>
+      </c>
+      <c r="E36" s="1">
+        <v>10119</v>
+      </c>
+      <c r="F36" s="14">
+        <f t="shared" si="4"/>
+        <v>16594.333403867102</v>
+      </c>
+      <c r="G36" s="14">
+        <f t="shared" si="5"/>
+        <v>82612.500330062918</v>
+      </c>
+      <c r="H36" s="1">
+        <v>878</v>
+      </c>
+      <c r="I36" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.6666730201223</v>
+      </c>
+      <c r="J36" s="1">
+        <v>228</v>
+      </c>
+      <c r="K36" s="14">
+        <f t="shared" si="7"/>
+        <v>350.83333277382263</v>
+      </c>
+      <c r="L36" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.5000057939449</v>
+      </c>
+      <c r="M36" s="1">
+        <v>34627</v>
+      </c>
+      <c r="N36" s="14">
+        <f t="shared" si="9"/>
+        <v>46721.333468278208</v>
+      </c>
+      <c r="O36" s="1">
+        <v>69470</v>
+      </c>
+      <c r="P36" s="14">
+        <f t="shared" si="10"/>
+        <v>98749.667014932507</v>
+      </c>
+      <c r="Q36" s="14">
+        <f t="shared" si="11"/>
+        <v>145471.00048321081</v>
+      </c>
+    </row>
+    <row r="37" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C37" s="1">
+        <v>125469</v>
+      </c>
+      <c r="D37" s="14">
+        <f t="shared" si="3"/>
+        <v>66018.166516172103</v>
+      </c>
+      <c r="E37" s="1">
+        <v>34586</v>
+      </c>
+      <c r="F37" s="14">
+        <f t="shared" si="4"/>
+        <v>16594.3333121305</v>
+      </c>
+      <c r="G37" s="14">
+        <f t="shared" si="5"/>
+        <v>82612.499828302607</v>
+      </c>
+      <c r="H37" s="1">
+        <v>3321</v>
+      </c>
+      <c r="I37" s="14">
+        <f t="shared" si="6"/>
+        <v>1460.6666634959045</v>
+      </c>
+      <c r="J37" s="1">
+        <v>862</v>
+      </c>
+      <c r="K37" s="14">
+        <f t="shared" si="7"/>
+        <v>350.8333339421003</v>
+      </c>
+      <c r="L37" s="14">
+        <f t="shared" si="8"/>
+        <v>1811.4999974380046</v>
+      </c>
+      <c r="M37" s="1">
+        <v>115185</v>
+      </c>
+      <c r="N37" s="14">
+        <f t="shared" si="9"/>
+        <v>46721.333292762109</v>
+      </c>
+      <c r="O37" s="1">
+        <v>222030</v>
+      </c>
+      <c r="P37" s="14">
+        <f t="shared" si="10"/>
+        <v>98749.666495906495</v>
+      </c>
+      <c r="Q37" s="14">
+        <f t="shared" si="11"/>
+        <v>145470.99978866871</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A50C8378-2448-425F-8964-BA1A083D5D21}">
+  <dimension ref="A1:L37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="35" customWidth="1"/>
+    <col min="7" max="7" width="34.28515625" customWidth="1"/>
+    <col min="8" max="8" width="36.5703125" customWidth="1"/>
+    <col min="9" max="9" width="29.28515625" customWidth="1"/>
+    <col min="10" max="10" width="27" customWidth="1"/>
+    <col min="11" max="12" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>2001</v>
+      </c>
+      <c r="C2" s="16">
+        <v>36892</v>
+      </c>
+      <c r="D2" s="1">
+        <v>66929</v>
+      </c>
+      <c r="E2" s="1">
+        <v>21562</v>
+      </c>
+      <c r="F2" s="1">
+        <v>88491</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1606</v>
+      </c>
+      <c r="H2" s="1">
+        <v>417</v>
+      </c>
+      <c r="I2" s="1">
+        <v>2023</v>
+      </c>
+      <c r="J2" s="1">
+        <v>56224</v>
+      </c>
+      <c r="K2" s="1">
+        <v>107446</v>
+      </c>
+      <c r="L2" s="1">
+        <v>163670</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>2001</v>
+      </c>
+      <c r="C3" s="16">
+        <v>36893</v>
+      </c>
+      <c r="D3" s="1">
+        <v>47890</v>
+      </c>
+      <c r="E3" s="1">
+        <v>11327</v>
+      </c>
+      <c r="F3" s="1">
+        <v>59217</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1008</v>
+      </c>
+      <c r="H3" s="1">
+        <v>385</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1393</v>
+      </c>
+      <c r="J3" s="1">
+        <v>36644</v>
+      </c>
+      <c r="K3" s="1">
+        <v>73884</v>
+      </c>
+      <c r="L3" s="1">
+        <v>110528</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>2001</v>
+      </c>
+      <c r="C4" s="16">
+        <v>36894</v>
+      </c>
+      <c r="D4" s="1">
+        <v>77800</v>
+      </c>
+      <c r="E4" s="1">
+        <v>18450</v>
+      </c>
+      <c r="F4" s="1">
+        <v>96250</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1714</v>
+      </c>
+      <c r="H4" s="1">
+        <v>306</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2020</v>
+      </c>
+      <c r="J4" s="1">
+        <v>50272</v>
+      </c>
+      <c r="K4" s="1">
+        <v>112428</v>
+      </c>
+      <c r="L4" s="1">
+        <v>162700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>2001</v>
+      </c>
+      <c r="C5" s="16">
+        <v>36895</v>
+      </c>
+      <c r="D5" s="1">
+        <v>64206.333333333336</v>
+      </c>
+      <c r="E5" s="1">
+        <v>17113</v>
+      </c>
+      <c r="F5" s="1">
+        <v>81319.333333333328</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1442.6666666666667</v>
+      </c>
+      <c r="H5" s="1">
+        <v>369.33333333333331</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1812</v>
+      </c>
+      <c r="J5" s="1">
+        <v>47713.333333333336</v>
+      </c>
+      <c r="K5" s="1">
+        <v>97919.333333333328</v>
+      </c>
+      <c r="L5" s="1">
+        <v>145632.66666666666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>2001</v>
+      </c>
+      <c r="C6" s="16">
+        <v>36896</v>
+      </c>
+      <c r="D6" s="1">
+        <v>63298.777777777781</v>
+      </c>
+      <c r="E6" s="1">
+        <v>15630</v>
+      </c>
+      <c r="F6" s="1">
+        <v>78928.777777777766</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1388.2222222222224</v>
+      </c>
+      <c r="H6" s="1">
+        <v>353.4444444444444</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1741.6666666666667</v>
+      </c>
+      <c r="J6" s="1">
+        <v>44876.444444444445</v>
+      </c>
+      <c r="K6" s="1">
+        <v>94743.777777777766</v>
+      </c>
+      <c r="L6" s="1">
+        <v>139620.22222222222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>2001</v>
+      </c>
+      <c r="C7" s="16">
+        <v>36897</v>
+      </c>
+      <c r="D7" s="1">
+        <v>68435.037037037036</v>
+      </c>
+      <c r="E7" s="1">
+        <v>17064.333333333332</v>
+      </c>
+      <c r="F7" s="1">
+        <v>85499.37037037035</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1514.9629629629633</v>
+      </c>
+      <c r="H7" s="1">
+        <v>342.92592592592587</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1857.8888888888889</v>
+      </c>
+      <c r="J7" s="1">
+        <v>47620.592592592591</v>
+      </c>
+      <c r="K7" s="1">
+        <v>101697.03703703702</v>
+      </c>
+      <c r="L7" s="1">
+        <v>149317.62962962964</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>2001</v>
+      </c>
+      <c r="C8" s="16">
+        <v>36898</v>
+      </c>
+      <c r="D8" s="1">
+        <v>65313.382716049382</v>
+      </c>
+      <c r="E8" s="1">
+        <v>16602.444444444442</v>
+      </c>
+      <c r="F8" s="1">
+        <v>81915.82716049382</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1448.6172839506173</v>
+      </c>
+      <c r="H8" s="1">
+        <v>355.23456790123447</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1803.851851851852</v>
+      </c>
+      <c r="J8" s="1">
+        <v>46736.790123456791</v>
+      </c>
+      <c r="K8" s="1">
+        <v>98120.049382716024</v>
+      </c>
+      <c r="L8" s="1">
+        <v>144856.83950617284</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>2001</v>
+      </c>
+      <c r="C9" s="16">
+        <v>36899</v>
+      </c>
+      <c r="D9" s="1">
+        <v>65682.399176954743</v>
+      </c>
+      <c r="E9" s="1">
+        <v>16432.259259259259</v>
+      </c>
+      <c r="F9" s="1">
+        <v>82114.658436213984</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1450.6008230452678</v>
+      </c>
+      <c r="H9" s="1">
+        <v>350.53497942386821</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1801.135802469136</v>
+      </c>
+      <c r="J9" s="1">
+        <v>46411.275720164609</v>
+      </c>
+      <c r="K9" s="1">
+        <v>98186.954732510261</v>
+      </c>
+      <c r="L9" s="1">
+        <v>144598.23045267491</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>2001</v>
+      </c>
+      <c r="C10" s="16">
+        <v>36900</v>
+      </c>
+      <c r="D10" s="1">
+        <v>66476.939643347054</v>
+      </c>
+      <c r="E10" s="1">
+        <v>16699.679012345678</v>
+      </c>
+      <c r="F10" s="1">
+        <v>83176.618655692713</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1471.3936899862829</v>
+      </c>
+      <c r="H10" s="1">
+        <v>349.56515775034285</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1820.9588477366258</v>
+      </c>
+      <c r="J10" s="1">
+        <v>46922.886145404664</v>
+      </c>
+      <c r="K10" s="1">
+        <v>99334.680384087769</v>
+      </c>
+      <c r="L10" s="1">
+        <v>146257.56652949247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>2001</v>
+      </c>
+      <c r="C11" s="16">
+        <v>36901</v>
+      </c>
+      <c r="D11" s="1">
+        <v>65824.24051211706</v>
+      </c>
+      <c r="E11" s="1">
+        <v>16578.127572016459</v>
+      </c>
+      <c r="F11" s="1">
+        <v>82402.368084133501</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1456.8705989940561</v>
+      </c>
+      <c r="H11" s="1">
+        <v>351.77823502514849</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1808.6488340192045</v>
+      </c>
+      <c r="J11" s="1">
+        <v>46690.317329675359</v>
+      </c>
+      <c r="K11" s="1">
+        <v>98547.228166438013</v>
+      </c>
+      <c r="L11" s="1">
+        <v>145237.54549611339</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>2001</v>
+      </c>
+      <c r="C12" s="16">
+        <v>36902</v>
+      </c>
+      <c r="D12" s="1">
+        <v>65994.526444139614</v>
+      </c>
+      <c r="E12" s="1">
+        <v>16570.0219478738</v>
+      </c>
+      <c r="F12" s="1">
+        <v>82564.548392013399</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1459.6217040085357</v>
+      </c>
+      <c r="H12" s="1">
+        <v>350.6261240664532</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1810.2478280749885</v>
+      </c>
+      <c r="J12" s="1">
+        <v>46674.82639841488</v>
+      </c>
+      <c r="K12" s="1">
+        <v>98689.621094345348</v>
+      </c>
+      <c r="L12" s="1">
+        <v>145364.44749276026</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <v>2001</v>
+      </c>
+      <c r="C13" s="16">
+        <v>36903</v>
+      </c>
+      <c r="D13" s="1">
+        <v>66098.568866534566</v>
+      </c>
+      <c r="E13" s="1">
+        <v>16615.942844078647</v>
+      </c>
+      <c r="F13" s="1">
+        <v>82714.511710613209</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1462.6286643296251</v>
+      </c>
+      <c r="H13" s="1">
+        <v>350.65650561398155</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1813.2851699436062</v>
+      </c>
+      <c r="J13" s="1">
+        <v>46762.676624498301</v>
+      </c>
+      <c r="K13" s="1">
+        <v>98857.176548290372</v>
+      </c>
+      <c r="L13" s="1">
+        <v>145619.85317278872</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>2001</v>
+      </c>
+      <c r="C14" s="16">
+        <v>36892</v>
+      </c>
+      <c r="D14" s="1">
+        <v>65972.445274263751</v>
+      </c>
+      <c r="E14" s="1">
+        <v>16588.030787989632</v>
+      </c>
+      <c r="F14" s="1">
+        <v>82560.476062253365</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1459.7069891107392</v>
+      </c>
+      <c r="H14" s="1">
+        <v>351.02028823519441</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1810.7272773459329</v>
+      </c>
+      <c r="J14" s="1">
+        <v>46709.273450862849</v>
+      </c>
+      <c r="K14" s="1">
+        <v>98698.008603024573</v>
+      </c>
+      <c r="L14" s="1">
+        <v>145407.28205388747</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <v>2001</v>
+      </c>
+      <c r="C15" s="16">
+        <v>36893</v>
+      </c>
+      <c r="D15" s="1">
+        <v>66021.846861645972</v>
+      </c>
+      <c r="E15" s="1">
+        <v>16591.331859980692</v>
+      </c>
+      <c r="F15" s="1">
+        <v>82613.178721626653</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1460.6524524829667</v>
+      </c>
+      <c r="H15" s="1">
+        <v>350.76763930520974</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1811.420091788176</v>
+      </c>
+      <c r="J15" s="1">
+        <v>46715.592157925341</v>
+      </c>
+      <c r="K15" s="1">
+        <v>98748.268748553426</v>
+      </c>
+      <c r="L15" s="1">
+        <v>145463.86090647883</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16">
+        <v>2001</v>
+      </c>
+      <c r="C16" s="16">
+        <v>36894</v>
+      </c>
+      <c r="D16" s="1">
+        <v>66030.95366748143</v>
+      </c>
+      <c r="E16" s="1">
+        <v>16598.435164016322</v>
+      </c>
+      <c r="F16" s="1">
+        <v>82629.388831497738</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1460.996035307777</v>
+      </c>
+      <c r="H16" s="1">
+        <v>350.8148110514619</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1811.8108463592382</v>
+      </c>
+      <c r="J16" s="1">
+        <v>46729.180744428828</v>
+      </c>
+      <c r="K16" s="1">
+        <v>98767.817966622781</v>
+      </c>
+      <c r="L16" s="1">
+        <v>145496.99871105168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <v>2001</v>
+      </c>
+      <c r="C17" s="16">
+        <v>36895</v>
+      </c>
+      <c r="D17" s="1">
+        <v>66008.415267797056</v>
+      </c>
+      <c r="E17" s="1">
+        <v>16592.599270662216</v>
+      </c>
+      <c r="F17" s="1">
+        <v>82601.014538459247</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1460.4518256338276</v>
+      </c>
+      <c r="H17" s="1">
+        <v>350.86757953062198</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1811.3194051644489</v>
+      </c>
+      <c r="J17" s="1">
+        <v>46718.015451072337</v>
+      </c>
+      <c r="K17" s="1">
+        <v>98738.031772733593</v>
+      </c>
+      <c r="L17" s="1">
+        <v>145456.047223806</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18">
+        <v>2001</v>
+      </c>
+      <c r="C18" s="16">
+        <v>36896</v>
+      </c>
+      <c r="D18" s="1">
+        <v>66020.405265641501</v>
+      </c>
+      <c r="E18" s="1">
+        <v>16594.122098219745</v>
+      </c>
+      <c r="F18" s="1">
+        <v>82614.527363861213</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1460.700104474857</v>
+      </c>
+      <c r="H18" s="1">
+        <v>350.81667662909786</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1811.5167811039544</v>
+      </c>
+      <c r="J18" s="1">
+        <v>46720.929451142169</v>
+      </c>
+      <c r="K18" s="1">
+        <v>98751.372829303262</v>
+      </c>
+      <c r="L18" s="1">
+        <v>145472.3022804455</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>2001</v>
+      </c>
+      <c r="C19" s="16">
+        <v>36897</v>
+      </c>
+      <c r="D19" s="1">
+        <v>66019.92473364</v>
+      </c>
+      <c r="E19" s="1">
+        <v>16595.052177632762</v>
+      </c>
+      <c r="F19" s="1">
+        <v>82614.976911272737</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1460.7159884721539</v>
+      </c>
+      <c r="H19" s="1">
+        <v>350.83302240372723</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1811.5490108758804</v>
+      </c>
+      <c r="J19" s="1">
+        <v>46722.708548881114</v>
+      </c>
+      <c r="K19" s="1">
+        <v>98752.40752288654</v>
+      </c>
+      <c r="L19" s="1">
+        <v>145475.11607176773</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20">
+        <v>2013</v>
+      </c>
+      <c r="C20" s="16">
+        <v>41275</v>
+      </c>
+      <c r="D20" s="1">
+        <v>66016.248422359524</v>
+      </c>
+      <c r="E20" s="1">
+        <v>16593.92451550491</v>
+      </c>
+      <c r="F20" s="1">
+        <v>82610.172937864394</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1460.6226395269462</v>
+      </c>
+      <c r="H20" s="1">
+        <v>350.83909285448232</v>
+      </c>
+      <c r="I20" s="1">
+        <v>1811.461732381428</v>
+      </c>
+      <c r="J20" s="1">
+        <v>46720.551150365209</v>
+      </c>
+      <c r="K20" s="1">
+        <v>98747.270708307798</v>
+      </c>
+      <c r="L20" s="1">
+        <v>145467.82185867309</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <v>2013</v>
+      </c>
+      <c r="C21" s="16">
+        <v>41276</v>
+      </c>
+      <c r="D21" s="1">
+        <v>66018.859473880337</v>
+      </c>
+      <c r="E21" s="1">
+        <v>16594.366263785807</v>
+      </c>
+      <c r="F21" s="1">
+        <v>82613.225737666115</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1460.6795774913189</v>
+      </c>
+      <c r="H21" s="1">
+        <v>350.82959729576913</v>
+      </c>
+      <c r="I21" s="1">
+        <v>1811.5091747870877</v>
+      </c>
+      <c r="J21" s="1">
+        <v>46721.39638346283</v>
+      </c>
+      <c r="K21" s="1">
+        <v>98750.350353499191</v>
+      </c>
+      <c r="L21" s="1">
+        <v>145471.74673696212</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22">
+        <v>2013</v>
+      </c>
+      <c r="C22" s="16">
+        <v>41277</v>
+      </c>
+      <c r="D22" s="1">
+        <v>66018.344209959949</v>
+      </c>
+      <c r="E22" s="1">
+        <v>16594.447652307827</v>
+      </c>
+      <c r="F22" s="1">
+        <v>82612.791862267753</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1460.6727351634729</v>
+      </c>
+      <c r="H22" s="1">
+        <v>350.83390418465956</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1811.506639348132</v>
+      </c>
+      <c r="J22" s="1">
+        <v>46721.552027569713</v>
+      </c>
+      <c r="K22" s="1">
+        <v>98750.009528231167</v>
+      </c>
+      <c r="L22" s="1">
+        <v>145471.56155580099</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23">
+        <v>2013</v>
+      </c>
+      <c r="C23" s="16">
+        <v>41278</v>
+      </c>
+      <c r="D23" s="1">
+        <v>66017.817368733275</v>
+      </c>
+      <c r="E23" s="1">
+        <v>16594.246143866181</v>
+      </c>
+      <c r="F23" s="1">
+        <v>82612.06351259943</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1460.6583173939125</v>
+      </c>
+      <c r="H23" s="1">
+        <v>350.83419811163702</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1811.4925155055491</v>
+      </c>
+      <c r="J23" s="1">
+        <v>46721.166520465915</v>
+      </c>
+      <c r="K23" s="1">
+        <v>98749.210196679385</v>
+      </c>
+      <c r="L23" s="1">
+        <v>145470.37671714541</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <v>2013</v>
+      </c>
+      <c r="C24" s="16">
+        <v>41279</v>
+      </c>
+      <c r="D24" s="1">
+        <v>66018.340350857863</v>
+      </c>
+      <c r="E24" s="1">
+        <v>16594.353353319937</v>
+      </c>
+      <c r="F24" s="1">
+        <v>82612.693704177756</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1460.6702100162347</v>
+      </c>
+      <c r="H24" s="1">
+        <v>350.83256653068861</v>
+      </c>
+      <c r="I24" s="1">
+        <v>1811.5027765469229</v>
+      </c>
+      <c r="J24" s="1">
+        <v>46721.371643832819</v>
+      </c>
+      <c r="K24" s="1">
+        <v>98749.856692803252</v>
+      </c>
+      <c r="L24" s="1">
+        <v>145471.22833663618</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25">
+        <v>2013</v>
+      </c>
+      <c r="C25" s="16">
+        <v>41280</v>
+      </c>
+      <c r="D25" s="1">
+        <v>66018.167309850352</v>
+      </c>
+      <c r="E25" s="1">
+        <v>16594.349049831315</v>
+      </c>
+      <c r="F25" s="1">
+        <v>82612.516359681656</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1460.66708752454</v>
+      </c>
+      <c r="H25" s="1">
+        <v>350.83355627566175</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1811.5006438002013</v>
+      </c>
+      <c r="J25" s="1">
+        <v>46721.363397289482</v>
+      </c>
+      <c r="K25" s="1">
+        <v>98749.692139237945</v>
+      </c>
+      <c r="L25" s="1">
+        <v>145471.05553652754</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26">
+        <v>2013</v>
+      </c>
+      <c r="C26" s="16">
+        <v>41281</v>
+      </c>
+      <c r="D26" s="1">
+        <v>66018.108343147163</v>
+      </c>
+      <c r="E26" s="1">
+        <v>16594.316182339146</v>
+      </c>
+      <c r="F26" s="1">
+        <v>82612.424525486291</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1460.665204978229</v>
+      </c>
+      <c r="H26" s="1">
+        <v>350.83344030599579</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1811.4986452842243</v>
+      </c>
+      <c r="J26" s="1">
+        <v>46721.30052052941</v>
+      </c>
+      <c r="K26" s="1">
+        <v>98749.586342906856</v>
+      </c>
+      <c r="L26" s="1">
+        <v>145470.88686343638</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27">
+        <v>2013</v>
+      </c>
+      <c r="C27" s="16">
+        <v>41282</v>
+      </c>
+      <c r="D27" s="1">
+        <v>66018.205334618455</v>
+      </c>
+      <c r="E27" s="1">
+        <v>16594.339528496799</v>
+      </c>
+      <c r="F27" s="1">
+        <v>82612.544863115239</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1460.6675008396678</v>
+      </c>
+      <c r="H27" s="1">
+        <v>350.83318770411535</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1811.5006885437826</v>
+      </c>
+      <c r="J27" s="1">
+        <v>46721.345187217237</v>
+      </c>
+      <c r="K27" s="1">
+        <v>98749.711724982699</v>
+      </c>
+      <c r="L27" s="1">
+        <v>145471.05691220003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28">
+        <v>2013</v>
+      </c>
+      <c r="C28" s="16">
+        <v>41283</v>
+      </c>
+      <c r="D28" s="1">
+        <v>66018.160329205319</v>
+      </c>
+      <c r="E28" s="1">
+        <v>16594.33492022242</v>
+      </c>
+      <c r="F28" s="1">
+        <v>82612.495249427724</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1460.6665977808123</v>
+      </c>
+      <c r="H28" s="1">
+        <v>350.83339476192424</v>
+      </c>
+      <c r="I28" s="1">
+        <v>1811.4999925427362</v>
+      </c>
+      <c r="J28" s="1">
+        <v>46721.336368345372</v>
+      </c>
+      <c r="K28" s="1">
+        <v>98749.663402375838</v>
+      </c>
+      <c r="L28" s="1">
+        <v>145470.9997707213</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29">
+        <v>2013</v>
+      </c>
+      <c r="C29" s="16">
+        <v>41284</v>
+      </c>
+      <c r="D29" s="1">
+        <v>66018.158002323646</v>
+      </c>
+      <c r="E29" s="1">
+        <v>16594.330210352786</v>
+      </c>
+      <c r="F29" s="1">
+        <v>82612.488212676428</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1460.6664345329029</v>
+      </c>
+      <c r="H29" s="1">
+        <v>350.83334092401179</v>
+      </c>
+      <c r="I29" s="1">
+        <v>1811.4997754569142</v>
+      </c>
+      <c r="J29" s="1">
+        <v>46721.327358697337</v>
+      </c>
+      <c r="K29" s="1">
+        <v>98749.653823421802</v>
+      </c>
+      <c r="L29" s="1">
+        <v>145470.98118211923</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30">
+        <v>2013</v>
+      </c>
+      <c r="C30" s="16">
+        <v>41285</v>
+      </c>
+      <c r="D30" s="1">
+        <v>66018.174555382473</v>
+      </c>
+      <c r="E30" s="1">
+        <v>16594.334886357334</v>
+      </c>
+      <c r="F30" s="1">
+        <v>82612.509441739807</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1460.666844384461</v>
+      </c>
+      <c r="H30" s="1">
+        <v>350.83330779668381</v>
+      </c>
+      <c r="I30" s="1">
+        <v>1811.5001521811444</v>
+      </c>
+      <c r="J30" s="1">
+        <v>46721.33630475332</v>
+      </c>
+      <c r="K30" s="1">
+        <v>98749.67631692678</v>
+      </c>
+      <c r="L30" s="1">
+        <v>145471.01262168019</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31">
+        <v>2013</v>
+      </c>
+      <c r="C31" s="16">
+        <v>41286</v>
+      </c>
+      <c r="D31" s="1">
+        <v>66018.164295637151</v>
+      </c>
+      <c r="E31" s="1">
+        <v>16594.333338977511</v>
+      </c>
+      <c r="F31" s="1">
+        <v>82612.497634614658</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1460.6666255660587</v>
+      </c>
+      <c r="H31" s="1">
+        <v>350.83334782753991</v>
+      </c>
+      <c r="I31" s="1">
+        <v>1811.4999733935983</v>
+      </c>
+      <c r="J31" s="1">
+        <v>46721.333343932005</v>
+      </c>
+      <c r="K31" s="1">
+        <v>98749.664514241464</v>
+      </c>
+      <c r="L31" s="1">
+        <v>145470.99785817356</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32">
+        <v>2013</v>
+      </c>
+      <c r="C32" s="16">
+        <v>41275</v>
+      </c>
+      <c r="D32" s="1">
+        <v>66018.165617781095</v>
+      </c>
+      <c r="E32" s="1">
+        <v>16594.332811895874</v>
+      </c>
+      <c r="F32" s="1">
+        <v>82612.498429676969</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1460.6666348278075</v>
+      </c>
+      <c r="H32" s="1">
+        <v>350.83333218274515</v>
+      </c>
+      <c r="I32" s="1">
+        <v>1811.4999670105524</v>
+      </c>
+      <c r="J32" s="1">
+        <v>46721.332335794221</v>
+      </c>
+      <c r="K32" s="1">
+        <v>98749.664884863349</v>
+      </c>
+      <c r="L32" s="1">
+        <v>145470.99722065765</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33">
+        <v>2013</v>
+      </c>
+      <c r="C33" s="16">
+        <v>41276</v>
+      </c>
+      <c r="D33" s="1">
+        <v>66018.168156266911</v>
+      </c>
+      <c r="E33" s="1">
+        <v>16594.333679076906</v>
+      </c>
+      <c r="F33" s="1">
+        <v>82612.501835343821</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1460.6667015927758</v>
+      </c>
+      <c r="H33" s="1">
+        <v>350.83332926898964</v>
+      </c>
+      <c r="I33" s="1">
+        <v>1811.5000308617653</v>
+      </c>
+      <c r="J33" s="1">
+        <v>46721.333994826513</v>
+      </c>
+      <c r="K33" s="1">
+        <v>98749.668572010531</v>
+      </c>
+      <c r="L33" s="1">
+        <v>145471.00256683712</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34">
+        <v>2013</v>
+      </c>
+      <c r="C34" s="16">
+        <v>41277</v>
+      </c>
+      <c r="D34" s="1">
+        <v>66018.16602322839</v>
+      </c>
+      <c r="E34" s="1">
+        <v>16594.333276650097</v>
+      </c>
+      <c r="F34" s="1">
+        <v>82612.499299878487</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1460.6666539955474</v>
+      </c>
+      <c r="H34" s="1">
+        <v>350.83333642642492</v>
+      </c>
+      <c r="I34" s="1">
+        <v>1811.4999904219721</v>
+      </c>
+      <c r="J34" s="1">
+        <v>46721.33322485091</v>
+      </c>
+      <c r="K34" s="1">
+        <v>98749.665990371781</v>
+      </c>
+      <c r="L34" s="1">
+        <v>145470.99921522278</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35">
+        <v>2013</v>
+      </c>
+      <c r="C35" s="16">
+        <v>41278</v>
+      </c>
+      <c r="D35" s="1">
+        <v>66018.166599092132</v>
+      </c>
+      <c r="E35" s="1">
+        <v>16594.333255874295</v>
+      </c>
+      <c r="F35" s="1">
+        <v>82612.499854966431</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1460.6666634720434</v>
+      </c>
+      <c r="H35" s="1">
+        <v>350.83333262605328</v>
+      </c>
+      <c r="I35" s="1">
+        <v>1811.4999960980967</v>
+      </c>
+      <c r="J35" s="1">
+        <v>46721.333185157215</v>
+      </c>
+      <c r="K35" s="1">
+        <v>98749.666482415225</v>
+      </c>
+      <c r="L35" s="1">
+        <v>145470.99966757253</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36">
+        <v>2013</v>
+      </c>
+      <c r="C36" s="16">
+        <v>41279</v>
+      </c>
+      <c r="D36" s="1">
+        <v>66018.166926195801</v>
+      </c>
+      <c r="E36" s="1">
+        <v>16594.333403867102</v>
+      </c>
+      <c r="F36" s="1">
+        <v>82612.500330062918</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1460.6666730201223</v>
+      </c>
+      <c r="H36" s="1">
+        <v>350.83333277382263</v>
+      </c>
+      <c r="I36" s="1">
+        <v>1811.5000057939449</v>
+      </c>
+      <c r="J36" s="1">
+        <v>46721.333468278208</v>
+      </c>
+      <c r="K36" s="1">
+        <v>98749.667014932507</v>
+      </c>
+      <c r="L36" s="1">
+        <v>145471.00048321081</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37">
+        <v>2013</v>
+      </c>
+      <c r="C37" s="16">
+        <v>41280</v>
+      </c>
+      <c r="D37" s="1">
+        <v>66018.166516172103</v>
+      </c>
+      <c r="E37" s="1">
+        <v>16594.3333121305</v>
+      </c>
+      <c r="F37" s="1">
+        <v>82612.499828302607</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1460.6666634959045</v>
+      </c>
+      <c r="H37" s="1">
+        <v>350.8333339421003</v>
+      </c>
+      <c r="I37" s="1">
+        <v>1811.4999974380046</v>
+      </c>
+      <c r="J37" s="1">
+        <v>46721.333292762109</v>
+      </c>
+      <c r="K37" s="1">
+        <v>98749.666495906495</v>
+      </c>
+      <c r="L37" s="1">
+        <v>145470.99978866871</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC629B83-ED03-47FE-B992-551FFAF657C6}">
   <dimension ref="B1:AC38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3914,6 +7527,9 @@
         <f t="shared" si="2"/>
         <v>542945921.43999982</v>
       </c>
+      <c r="J14" t="s">
+        <v>75</v>
+      </c>
       <c r="L14">
         <f>_xlfn.STDEV.S(C2:C37)</f>
         <v>44925.518945929951</v>
@@ -3941,6 +7557,12 @@
         <f t="shared" si="2"/>
         <v>695176502.43999982</v>
       </c>
+      <c r="J15" t="s">
+        <v>63</v>
+      </c>
+      <c r="K15">
+        <v>990</v>
+      </c>
       <c r="L15">
         <f>AVERAGE(C2:C37)</f>
         <v>30710.805555555555</v>
@@ -3968,6 +7590,12 @@
         <f t="shared" si="2"/>
         <v>245273185.43999991</v>
       </c>
+      <c r="J16" t="s">
+        <v>64</v>
+      </c>
+      <c r="K16">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="17" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B17">
@@ -3987,6 +7615,12 @@
       <c r="F17">
         <f t="shared" si="2"/>
         <v>293957883.0399999</v>
+      </c>
+      <c r="J17" t="s">
+        <v>65</v>
+      </c>
+      <c r="K17">
+        <v>0.4</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>71</v>

</xml_diff>